<commit_message>
update files to 20230718002732
</commit_message>
<xml_diff>
--- a/phase/tmc_img/Shopee Images_Tap Hoa Toc Do_hws.xlsx
+++ b/phase/tmc_img/Shopee Images_Tap Hoa Toc Do_hws.xlsx
@@ -1,22 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Go XLSX"/>
-  <workbookPr showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\bash-script\phase\tmc_img\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790DD8D7-A131-48AA-942A-6630F112096C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" tabRatio="204" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="24980" yWindow="0" windowWidth="13510" windowHeight="20970" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Image" sheetId="1" r:id="rId1" state="visible"/>
+    <sheet name="Image" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr iterateCount="100" refMode="A1" iterateDelta="0.001"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="220">
   <si>
     <t>Tên tập tin đa phương tiện</t>
   </si>
@@ -681,64 +698,86 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
-      <family val="0"/>
-      <charset val="0"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <name val="Verdana"/>
-      <family val="0"/>
-      <charset val="0"/>
-      <b/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="00000000"/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="2">
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
   <cellXfs count="3">
-    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="2" fontId="1" numFmtId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1063,1499 +1102,1500 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="A1:D105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.5"/>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="58.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
         <v>85</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>91</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
         <v>92</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
         <v>94</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>98</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
         <v>99</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
         <v>101</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
         <v>103</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>98</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
         <v>105</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>100</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>81</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>95</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
         <v>109</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>87</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
         <v>110</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>112</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
         <v>113</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>114</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="1" t="s">
+      <c r="B49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" t="s">
         <v>115</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>116</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
         <v>117</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>119</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="1" t="s">
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
         <v>120</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>121</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>123</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="1" t="s">
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
         <v>124</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>125</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
         <v>126</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>127</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
         <v>128</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>130</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
         <v>131</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>132</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C57" s="1" t="s">
+      <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
         <v>133</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>134</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="1" t="s">
+      <c r="B58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s">
         <v>135</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>136</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="1" t="s">
+      <c r="B59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
         <v>137</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="B60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
         <v>138</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>139</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="1" t="s">
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
         <v>140</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>141</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" s="1" t="s">
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
         <v>142</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>143</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" s="1" t="s">
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
         <v>144</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>145</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" s="1" t="s">
+      <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s">
         <v>146</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>147</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C65" s="1" t="s">
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" t="s">
         <v>148</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>149</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" s="1" t="s">
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" t="s">
         <v>150</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>151</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C67" s="1" t="s">
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
         <v>152</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>153</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C68" s="1" t="s">
+      <c r="B68" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
         <v>154</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>155</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="1" t="s">
+      <c r="B69" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s">
         <v>156</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>158</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="1" t="s">
+      <c r="B70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" t="s">
         <v>159</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>161</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="1" t="s">
+      <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" t="s">
         <v>162</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>164</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="1" t="s">
+      <c r="B72" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" t="s">
         <v>165</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>167</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="1" t="s">
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" t="s">
         <v>168</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>170</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" s="1" t="s">
+      <c r="B74" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" t="s">
         <v>171</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>141</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="1" t="s">
+      <c r="B75" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" t="s">
         <v>172</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>127</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="1" t="s">
+      <c r="B76" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" t="s">
         <v>174</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D76" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>176</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="1" t="s">
+      <c r="B77" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" t="s">
         <v>177</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>178</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="1" t="s">
+      <c r="B78" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" t="s">
         <v>179</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D78" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>119</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79" s="1" t="s">
+      <c r="B79" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" t="s">
         <v>180</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D79" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>181</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" s="1" t="s">
+      <c r="B80" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" t="s">
         <v>182</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D80" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>184</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="1" t="s">
+      <c r="B81" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" t="s">
         <v>185</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D81" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>136</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" s="1" t="s">
+      <c r="B82" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" t="s">
         <v>186</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D82" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" s="1" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>149</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C83" s="1" t="s">
+      <c r="B83" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" t="s">
         <v>187</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D83" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>132</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" s="1" t="s">
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D84" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" s="1" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>123</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="1" t="s">
+      <c r="B85" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" t="s">
         <v>189</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D85" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>143</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" s="1" t="s">
+      <c r="B86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" t="s">
         <v>190</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D86" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" s="1" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>145</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C87" s="1" t="s">
+      <c r="B87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" t="s">
         <v>191</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D87" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>192</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="1" t="s">
+      <c r="B88" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" t="s">
         <v>193</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D88" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" s="1" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>194</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="1" t="s">
+      <c r="B89" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" t="s">
         <v>195</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D89" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>130</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="1" t="s">
+      <c r="B90" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" t="s">
         <v>196</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D90" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" s="1" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>139</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="1" t="s">
+      <c r="B91" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" t="s">
         <v>197</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D91" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" s="1" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>164</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="1" t="s">
+      <c r="B92" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" t="s">
         <v>199</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D92" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" s="1" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>136</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" s="1" t="s">
+      <c r="B93" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" t="s">
         <v>201</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D93" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" s="1" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>153</v>
       </c>
-      <c r="B94" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C94" s="1" t="s">
+      <c r="B94" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" t="s">
         <v>203</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D94" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" s="1" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>130</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C95" s="1" t="s">
+      <c r="B95" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" t="s">
         <v>205</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D95" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" s="1" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>151</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C96" s="1" t="s">
+      <c r="B96" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" t="s">
         <v>207</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D96" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="97">
-      <c r="A97" s="1" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>123</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" s="1" t="s">
+      <c r="B97" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" t="s">
         <v>208</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D97" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" s="1" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>192</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" s="1" t="s">
+      <c r="B98" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" t="s">
         <v>209</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="D98" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" s="1" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>149</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C99" s="1" t="s">
+      <c r="B99" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" t="s">
         <v>210</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D99" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" s="1" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>194</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" s="1" t="s">
+      <c r="B100" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" t="s">
         <v>211</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D100" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" s="1" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>181</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" s="1" t="s">
+      <c r="B101" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" t="s">
         <v>212</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D101" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="102">
-      <c r="A102" s="1" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>213</v>
       </c>
-      <c r="B102" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C102" s="1" t="s">
+      <c r="B102" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" t="s">
         <v>214</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="D102" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" s="1" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>215</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C103" s="1" t="s">
+      <c r="B103" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" t="s">
         <v>216</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="D103" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="104">
-      <c r="A104" s="1" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>134</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C104" s="1" t="s">
+      <c r="B104" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" t="s">
         <v>217</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D104" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="105">
-      <c r="A105" s="1" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>143</v>
       </c>
-      <c r="B105" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C105" s="1" t="s">
+      <c r="B105" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" t="s">
         <v>218</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D105" t="s">
         <v>219</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <hyperlinks>
+    <hyperlink ref="C52" r:id="rId1" xr:uid="{FBEFCF2C-47EF-4A69-BC4F-4D8F3BC8AAAB}"/>
+    <hyperlink ref="C84" r:id="rId2" xr:uid="{37514B29-37FC-476A-9A9A-B084CF867F98}"/>
+  </hyperlinks>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="256" orientation="portrait" useFirstPageNumber="1" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>